<commit_message>
fixes own IHS interchange
</commit_message>
<xml_diff>
--- a/peer_review_2024.xlsx
+++ b/peer_review_2024.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11520" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="11500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Self Responses" sheetId="1" r:id="rId1"/>
@@ -534,12 +534,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -598,6 +598,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -605,13 +610,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -625,10 +633,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -649,22 +673,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -678,7 +701,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -701,7 +724,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -709,32 +732,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -759,37 +759,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,7 +789,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,19 +813,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,7 +831,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,13 +849,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,13 +873,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,7 +885,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,19 +897,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,13 +915,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -950,6 +950,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1017,173 +1050,140 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1193,7 +1193,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1202,7 +1202,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1302,13 +1302,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -9923,10 +9923,10 @@
   <sheetPr/>
   <dimension ref="A1:O326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="12"/>
@@ -13152,17 +13152,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AG998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="26.1160714285714" customWidth="1"/>
+    <col min="3" max="3" width="22.6071428571429" customWidth="1"/>
+    <col min="4" max="4" width="24.5535714285714" customWidth="1"/>
+    <col min="16" max="16" width="35.1160714285714" customWidth="1"/>
     <col min="19" max="21" width="12.3839285714286" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>